<commit_message>
removed bio-oil production in biochar land scenario and updated plant costs
</commit_message>
<xml_diff>
--- a/gcam-sandbox/input/gcamdata/plant_costs.xlsx
+++ b/gcam-sandbox/input/gcamdata/plant_costs.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\gcam-sandbox\input\gcamdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\drawing_figures\gcam-sandbox\input\gcamdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ECA50B-AA10-47EC-ABE1-96D833E4B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E339F03-78E1-4351-95E5-276E04BC574F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pyrolysis-nofert" sheetId="1" r:id="rId1"/>
+    <sheet name="biochar_land" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>hrs/day</t>
   </si>
@@ -147,6 +148,12 @@
   </si>
   <si>
     <t>Yield (kg/GJ)</t>
+  </si>
+  <si>
+    <t>same as beef/dairy</t>
+  </si>
+  <si>
+    <t>Unit cost  ($1975/kg)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +487,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +943,435 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
       <c r="E26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C229AC-139E-41F1-AA79-F61EE8EC5D09}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>330</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>1/2.1815</f>
+        <v>0.45840018336007332</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f>1/2.1052</f>
+        <v>0.47501425042751283</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f>1/2.055</f>
+        <v>0.48661800486618001</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f>1/2.136</f>
+        <v>0.46816479400749061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f>1/2.1276</f>
+        <v>0.47001316036849028</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>40.8*($A$1*1000)^0.6194</f>
+        <v>5812.8493587040821</v>
+      </c>
+      <c r="C13">
+        <f>0.09*B13+(1.04*$A$1)^0.475/(1+0.07)</f>
+        <v>524.76094203599132</v>
+      </c>
+      <c r="D13" s="4">
+        <f>-PV(7%,30,C13)+B13</f>
+        <v>12324.629499924029</v>
+      </c>
+      <c r="E13" s="4">
+        <f>D13*1000/0.9233*0.32</f>
+        <v>4271505.9460367039</v>
+      </c>
+      <c r="F13" s="4">
+        <f>-PMT(7%, 30,E13)</f>
+        <v>344225.30176742456</v>
+      </c>
+      <c r="G13">
+        <f>A$1*A$2*A$3*A4*A$9</f>
+        <v>10891588.356635341</v>
+      </c>
+      <c r="H13" s="5">
+        <f>F13/G13</f>
+        <v>3.1604692584412321E-2</v>
+      </c>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>40.8*($A$1*1000)^0.6194</f>
+        <v>5812.8493587040821</v>
+      </c>
+      <c r="C14">
+        <f>0.09*B14+(1.04*$A$1)^0.475/(1+0.07)</f>
+        <v>524.76094203599132</v>
+      </c>
+      <c r="D14" s="4">
+        <f>-PV(7%,30,C14)+B14</f>
+        <v>12324.629499924029</v>
+      </c>
+      <c r="E14" s="4">
+        <f>D14*1000/0.9233*0.32</f>
+        <v>4271505.9460367039</v>
+      </c>
+      <c r="F14" s="4">
+        <f>-PMT(7%, 30,E14)</f>
+        <v>344225.30176742456</v>
+      </c>
+      <c r="G14">
+        <f>A$1*A$2*A$3*A5*A$9</f>
+        <v>11286338.590157704</v>
+      </c>
+      <c r="H14" s="5">
+        <f>F14/G14</f>
+        <v>3.0499288942793863E-2</v>
+      </c>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>40.8*($A$1*1000)^0.6194</f>
+        <v>5812.8493587040821</v>
+      </c>
+      <c r="C15">
+        <f>0.09*B15+(1.04*$A$1)^0.475/(1+0.07)</f>
+        <v>524.76094203599132</v>
+      </c>
+      <c r="D15" s="4">
+        <f>-PV(7%,30,C15)+B15</f>
+        <v>12324.629499924029</v>
+      </c>
+      <c r="E15" s="4">
+        <f>D15*1000/0.9233*0.32</f>
+        <v>4271505.9460367039</v>
+      </c>
+      <c r="F15" s="4">
+        <f>-PMT(7%, 30,E15)</f>
+        <v>344225.30176742456</v>
+      </c>
+      <c r="G15">
+        <f>A$1*A$2*A$3*A6*A$9</f>
+        <v>11562043.795620438</v>
+      </c>
+      <c r="H15" s="5">
+        <f>F15/G15</f>
+        <v>2.9772011579632048E-2</v>
+      </c>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>40.8*($A$1*1000)^0.6194</f>
+        <v>5812.8493587040821</v>
+      </c>
+      <c r="C16">
+        <f>0.09*B16+(1.04*$A$1)^0.475/(1+0.07)</f>
+        <v>524.76094203599132</v>
+      </c>
+      <c r="D16" s="4">
+        <f>-PV(7%,30,C16)+B16</f>
+        <v>12324.629499924029</v>
+      </c>
+      <c r="E16" s="4">
+        <f>D16*1000/0.9233*0.32</f>
+        <v>4271505.9460367039</v>
+      </c>
+      <c r="F16" s="4">
+        <f>-PMT(7%, 30,E16)</f>
+        <v>344225.30176742456</v>
+      </c>
+      <c r="G16">
+        <f>A$1*A$2*A$3*A7*A$9</f>
+        <v>11123595.505617978</v>
+      </c>
+      <c r="H16" s="5">
+        <f>F16/G16</f>
+        <v>3.094550692656645E-2</v>
+      </c>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f>40.8*($A$1*1000)^0.6194</f>
+        <v>5812.8493587040821</v>
+      </c>
+      <c r="C17">
+        <f>0.09*B17+(1.04*$A$1)^0.475/(1+0.07)</f>
+        <v>524.76094203599132</v>
+      </c>
+      <c r="D17" s="4">
+        <f>-PV(7%,30,C17)+B17</f>
+        <v>12324.629499924029</v>
+      </c>
+      <c r="E17" s="4">
+        <f>D17*1000/0.9233*0.32</f>
+        <v>4271505.9460367039</v>
+      </c>
+      <c r="F17" s="4">
+        <f>-PMT(7%, 30,E17)</f>
+        <v>344225.30176742456</v>
+      </c>
+      <c r="G17">
+        <f>A$1*A$2*A$3*A8*A$9</f>
+        <v>11167512.690355329</v>
+      </c>
+      <c r="H17" s="5">
+        <f>F17/G17</f>
+        <v>3.0823811112810292E-2</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1630000000</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1230000000</v>
+      </c>
+      <c r="D21">
+        <v>94</v>
+      </c>
+      <c r="E21" s="7">
+        <f>(B21+C21)/(D21*1000000)</f>
+        <v>30.425531914893618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2760000000</v>
+      </c>
+      <c r="C22" s="7">
+        <v>901000000</v>
+      </c>
+      <c r="D22">
+        <v>63</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" ref="E22:E24" si="0">(B22+C22)/(D22*1000000)</f>
+        <v>58.111111111111114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="7">
+        <v>4700000000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>3330000000</v>
+      </c>
+      <c r="D23">
+        <v>294</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>27.312925170068027</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="7">
+        <v>4700000000</v>
+      </c>
+      <c r="C24" s="7">
+        <v>3330000000</v>
+      </c>
+      <c r="D24">
+        <v>294</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>27.312925170068027</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated R files for biochar land nodes
</commit_message>
<xml_diff>
--- a/gcam-sandbox/input/gcamdata/plant_costs.xlsx
+++ b/gcam-sandbox/input/gcamdata/plant_costs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\drawing_figures\gcam-sandbox\input\gcamdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E339F03-78E1-4351-95E5-276E04BC574F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CEEA33-C5AD-4698-8600-EC853EB970A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyrolysis-nofert" sheetId="1" r:id="rId1"/>
     <sheet name="biochar_land" sheetId="2" r:id="rId2"/>
+    <sheet name="gompertz" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>hrs/day</t>
   </si>
@@ -154,6 +155,27 @@
   </si>
   <si>
     <t>Unit cost  ($1975/kg)</t>
+  </si>
+  <si>
+    <t>B_max</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Time Period</t>
+  </si>
+  <si>
+    <t>(4 years from 2024)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1377,4 +1399,641 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248186C2-819E-40A3-BDA6-AECDD5B5B57C}">
+  <dimension ref="A1:Y11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1">
+        <v>1975</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2020</v>
+      </c>
+      <c r="J1">
+        <v>2025</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2035</v>
+      </c>
+      <c r="M1">
+        <v>2040</v>
+      </c>
+      <c r="N1">
+        <v>2045</v>
+      </c>
+      <c r="O1">
+        <v>2050</v>
+      </c>
+      <c r="P1">
+        <v>2055</v>
+      </c>
+      <c r="Q1">
+        <v>2060</v>
+      </c>
+      <c r="R1">
+        <v>2065</v>
+      </c>
+      <c r="S1">
+        <v>2070</v>
+      </c>
+      <c r="T1">
+        <v>2075</v>
+      </c>
+      <c r="U1">
+        <v>2080</v>
+      </c>
+      <c r="V1">
+        <v>2085</v>
+      </c>
+      <c r="W1">
+        <v>2090</v>
+      </c>
+      <c r="X1">
+        <v>2095</v>
+      </c>
+      <c r="Y1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>9</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <v>13</v>
+      </c>
+      <c r="U2">
+        <v>14</v>
+      </c>
+      <c r="V2">
+        <v>15</v>
+      </c>
+      <c r="W2">
+        <v>16</v>
+      </c>
+      <c r="X2">
+        <v>17</v>
+      </c>
+      <c r="Y2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2.589</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+      <c r="E3">
+        <v>2028</v>
+      </c>
+      <c r="G3">
+        <f>IF($B3*EXP(-$C3*EXP(-$D3*(G$1-$E3))) &lt; 0.001, 0, $B3*EXP(-$C3*EXP(-$D3*(G$1-$E3))))</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>IF($B3*EXP(-$C3*EXP(-$D3*(H$1-$E3))) &lt; 0.001, 0, $B3*EXP(-$C3*EXP(-$D3*(H$1-$E3))))</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:Y7" si="0">IF($B3*EXP(-$C3*EXP(-$D3*(I$1-$E3))) &lt; 0.001, 0, $B3*EXP(-$C3*EXP(-$D3*(I$1-$E3))))</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>3.2778565663512398E-3</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>0.38280036068115975</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>1.4972258294302512</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>2.2130355558960431</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>2.4751901341438214</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>2.5558683398063873</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>2.579463965049178</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="0"/>
+        <v>2.586264282654485</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
+        <v>2.5882159082160339</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>2.5887753296671216</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>2.5889356288790717</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="0"/>
+        <v>2.5889815572014876</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="0"/>
+        <v>2.5889947160363307</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="0"/>
+        <v>2.5889984861179602</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="0"/>
+        <v>2.5889995662654433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.453592</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0.25</v>
+      </c>
+      <c r="E4">
+        <v>2028</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:V7" si="1">IF($B4*EXP(-$C4*EXP(-$D4*(G$1-$E4))) &lt; 0.001, 0, $B4*EXP(-$C4*EXP(-$D4*(G$1-$E4))))</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>6.7066504906175592E-2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>0.26231350267397702</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>0.3877231455658548</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>0.43365254666920211</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>0.44778734337174925</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>0.45192128962324707</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>0.45311270316640134</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="1"/>
+        <v>0.4534546273617332</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>0.45355263782710281</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="1"/>
+        <v>0.45358072219950402</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="1"/>
+        <v>0.4535887688273994</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>0.45359107425119788</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>0.45359173476833436</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>0.45359192400983966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>3.101</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0.25</v>
+      </c>
+      <c r="E5">
+        <v>2028</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>3.9260846706277303E-3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.45850286538133506</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1.7933168393446151</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>2.6506849203683394</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>2.9646831232058672</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>3.0613162308766344</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>3.0895781211346081</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>3.0977232678685045</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>3.1000608464186636</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>3.1007308989176305</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>3.1009228988621094</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>3.1009779099582127</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>3.1009936710809813</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>3.1009981867330221</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>3.1009994804902044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0.25</v>
+      </c>
+      <c r="E6">
+        <v>2028</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>4.4948362165729075E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.17580403713665366</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.25985431015542571</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0.2906364622555897</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.30010968532295934</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0.30288028017572421</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>0.30367877247082403</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>0.30390793205781158</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>0.30397361924248939</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>0.30399244155242866</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>0.30399783444930562</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>0.30399937955776146</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>0.30399982224019306</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>0.30399994907095201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1.381</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0.25</v>
+      </c>
+      <c r="E7">
+        <v>2028</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.7484433828238942E-3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.20418976365418373</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.79863610291354836</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1.18045658659422</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>1.3202926130755572</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1.3633272218125225</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>1.3759133780351156</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>1.379540739415158</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>1.3805817571442034</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1.3808801584667034</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>1.380965663762842</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>1.380990162416089</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>1.3809971814778572</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>1.3809991924792981</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>1.3809997686413971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>-$C3*EXP(-$D3*G$1-$E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>EXP(-$D3*G$1-$E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f>-$D3*G$1-$E3</f>
+        <v>-2521.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>